<commit_message>
excelBD.py atualizada para alimentar BDs
</commit_message>
<xml_diff>
--- a/public/colaborador_treinamentos.xlsx
+++ b/public/colaborador_treinamentos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t xml:space="preserve">colaborador_id</t>
   </si>
@@ -54,7 +54,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -88,11 +88,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,7 +132,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -154,28 +149,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -304,7 +287,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -333,10 +316,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>44941</v>
@@ -350,10 +333,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>44602</v>
@@ -367,10 +350,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>44275</v>
@@ -384,10 +367,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>44691</v>
@@ -401,10 +384,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>44336</v>
@@ -418,18 +401,18 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="B7" s="6" t="n">
-        <v>16</v>
-      </c>
-      <c r="C7" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4" t="n">
         <v>44941</v>
       </c>
-      <c r="D7" s="8" t="n">
-        <v>45672</v>
-      </c>
-      <c r="E7" s="9" t="s">
+      <c r="D7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>